<commit_message>
Added locations and multiple images
</commit_message>
<xml_diff>
--- a/test/HWDBUtility/SystemTest/flapdoodle/Items.xlsx
+++ b/test/HWDBUtility/SystemTest/flapdoodle/Items.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -61,16 +61,16 @@
     <t xml:space="preserve">child</t>
   </si>
   <si>
-    <t xml:space="preserve">SN990005</t>
+    <t xml:space="preserve">SN990008</t>
   </si>
   <si>
     <t xml:space="preserve">testing self-subcomponent</t>
   </si>
   <si>
-    <t xml:space="preserve">SN990006</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SN990007</t>
+    <t xml:space="preserve">SN990009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SN990010</t>
   </si>
 </sst>
 </file>
@@ -85,6 +85,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -102,13 +103,13 @@
       <family val="0"/>
     </font>
     <font>
-      <b val="true"/>
       <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -165,15 +166,15 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
@@ -182,15 +183,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -210,9 +211,9 @@
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="key" xfId="20"/>
-    <cellStyle name="data" xfId="21"/>
-    <cellStyle name="header_data" xfId="22"/>
+    <cellStyle name="data" xfId="20"/>
+    <cellStyle name="header_data" xfId="21"/>
+    <cellStyle name="key" xfId="22"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -225,10 +226,10 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.52"/>

</xml_diff>

<commit_message>
app now outputs a summary sheet of items uploaded
</commit_message>
<xml_diff>
--- a/test/HWDBUtility/SystemTest/flapdoodle/Items.xlsx
+++ b/test/HWDBUtility/SystemTest/flapdoodle/Items.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t xml:space="preserve">Record Type</t>
   </si>
@@ -58,19 +58,19 @@
     <t xml:space="preserve">Comments</t>
   </si>
   <si>
-    <t xml:space="preserve">child</t>
-  </si>
-  <si>
     <t xml:space="preserve">SN990008</t>
   </si>
   <si>
-    <t xml:space="preserve">testing self-subcomponent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SN990009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SN990010</t>
+    <t xml:space="preserve">testing output sheets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SN990102</t>
+  </si>
+  <si>
+    <t xml:space="preserve">new</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SN990103</t>
   </si>
 </sst>
 </file>
@@ -226,10 +226,10 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.52"/>
@@ -328,42 +328,34 @@
       <c r="B7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>12</v>
-      </c>
+      <c r="C7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>15</v>
-      </c>
+      <c r="C8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>16</v>
-      </c>
+      <c r="C9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="C10" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>